<commit_message>
début query pour les armes
</commit_message>
<xml_diff>
--- a/docs/B65_-_Hiver_2019_-_Outil_de_planification_et_de_suivi_de_projet.xlsx
+++ b/docs/B65_-_Hiver_2019_-_Outil_de_planification_et_de_suivi_de_projet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ecole\synthese\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF795469-238B-44B1-8C3A-69E18718B59A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288E4A05-841A-4E10-8A72-F9E92E03C88A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="494" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="99">
   <si>
     <t>No</t>
   </si>
@@ -478,6 +478,12 @@
   </si>
   <si>
     <t>Exporter les vraies données du jeu</t>
+  </si>
+  <si>
+    <t>Il reste quelques petites choses à fixer dans le parseur</t>
+  </si>
+  <si>
+    <t>pas eu le temps</t>
   </si>
 </sst>
 </file>
@@ -1549,6 +1555,53 @@
   </cellStyles>
   <dxfs count="82">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDEEEF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <top style="thin">
+          <color rgb="FFC00000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFC00000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFF40000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF1F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00C000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE5FFE5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1707,13 +1760,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFEDEEEF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="0"/>
         </patternFill>
       </fill>
@@ -1755,26 +1801,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <top style="thin">
-          <color rgb="FFC00000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFC00000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FFE00000"/>
       </font>
@@ -1791,26 +1817,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFD1FFD1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFF40000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF1F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00C000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE5FFE5"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3251,7 +3257,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3677,10 +3683,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3794,10 +3800,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4256,10 +4262,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7049,7 +7055,7 @@
   <dimension ref="B1:AJ90"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7860,7 +7866,7 @@
         <v>14</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F18" s="18">
         <v>3</v>
@@ -7946,7 +7952,7 @@
         <v>14</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F19" s="16">
         <v>2</v>
@@ -8026,7 +8032,7 @@
         <v>14</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F20" s="18">
         <v>2</v>
@@ -11050,7 +11056,7 @@
   <dimension ref="B1:Z57"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11115,7 +11121,7 @@
       <c r="H5" s="34"/>
       <c r="I5" s="63" t="str">
         <f>IF(M45=0,CONCATENATE("Ce sprint totalise ", W15, " de travail réalisé. ",W16),CONCATENATE("Attention, il reste ",M46," à remplir!"))</f>
-        <v>Attention, il reste 11 champs à remplir!</v>
+        <v>Ce sprint totalise 18 heures de travail réalisé. 6 tâches sont en retard!</v>
       </c>
     </row>
     <row r="6" spans="2:25" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -11212,7 +11218,7 @@
       </c>
       <c r="V9" s="9">
         <f>SUM(G9:G43)</f>
-        <v>0.66666666666666818</v>
+        <v>0.75000000000000133</v>
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.25">
@@ -11260,15 +11266,15 @@
       </c>
       <c r="S10" s="60">
         <f t="array" ref="S10">SUM(($D$9:$D$43=$R10)*$G$9:$G$43)</f>
-        <v>0.66666666666666818</v>
+        <v>0.75000000000000133</v>
       </c>
       <c r="T10" s="61">
         <f t="shared" ref="T10:T11" si="4">S10*24*60</f>
-        <v>960.00000000000216</v>
+        <v>1080.0000000000018</v>
       </c>
       <c r="V10" s="10">
         <f>V9</f>
-        <v>0.66666666666666818</v>
+        <v>0.75000000000000133</v>
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.25">
@@ -11324,7 +11330,7 @@
       </c>
       <c r="V11" s="62">
         <f>DAY(V9)*24+HOUR(V9)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
@@ -11396,7 +11402,7 @@
         <v/>
       </c>
       <c r="G13" s="116">
-        <v>4.1666666666666699E-2</v>
+        <v>8.3333333333333301E-2</v>
       </c>
       <c r="H13" s="114">
         <v>1</v>
@@ -11424,11 +11430,11 @@
       </c>
       <c r="V13" s="62">
         <f>V11</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="W13" s="4" t="str">
         <f>V13 &amp; " " &amp; U13 &amp; IF(V13 &gt; 1, "s", "")</f>
-        <v>16 heures</v>
+        <v>18 heures</v>
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
@@ -11510,7 +11516,7 @@
         <v/>
       </c>
       <c r="G15" s="116">
-        <v>4.1666666666666699E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H15" s="114">
         <v>1</v>
@@ -11535,11 +11541,11 @@
       <c r="R15" s="8"/>
       <c r="W15" s="4" t="str">
         <f>IF(V13&gt;0,IF(V14&gt;0,W13&amp;" et "&amp;W14,W13),W14)</f>
-        <v>16 heures</v>
+        <v>18 heures</v>
       </c>
       <c r="Y15" s="4" t="str">
         <f>V13&amp;"h"&amp;TEXT(V14,"00")</f>
-        <v>16h00</v>
+        <v>18h00</v>
       </c>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
@@ -11569,7 +11575,9 @@
       <c r="H16" s="111">
         <v>0.8</v>
       </c>
-      <c r="I16" s="112"/>
+      <c r="I16" s="112" t="s">
+        <v>97</v>
+      </c>
       <c r="M16" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -11580,7 +11588,7 @@
       </c>
       <c r="O16" s="3" t="b">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16" s="3" t="b">
         <f t="shared" si="3"/>
@@ -11617,16 +11625,22 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F16),"",'Sprint 1 - Bilan'!F16)</f>
         <v/>
       </c>
-      <c r="G17" s="113"/>
-      <c r="H17" s="114"/>
-      <c r="I17" s="115"/>
+      <c r="G17" s="113">
+        <v>0</v>
+      </c>
+      <c r="H17" s="114">
+        <v>0</v>
+      </c>
+      <c r="I17" s="115" t="s">
+        <v>98</v>
+      </c>
       <c r="M17" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11659,16 +11673,22 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F17),"",'Sprint 1 - Bilan'!F17)</f>
         <v/>
       </c>
-      <c r="G18" s="110"/>
-      <c r="H18" s="111"/>
-      <c r="I18" s="112"/>
+      <c r="G18" s="110">
+        <v>0</v>
+      </c>
+      <c r="H18" s="111">
+        <v>0</v>
+      </c>
+      <c r="I18" s="115" t="s">
+        <v>98</v>
+      </c>
       <c r="M18" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O18" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11701,17 +11721,23 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F18),"",'Sprint 1 - Bilan'!F18)</f>
         <v/>
       </c>
-      <c r="G19" s="116"/>
-      <c r="H19" s="114"/>
-      <c r="I19" s="115"/>
+      <c r="G19" s="116">
+        <v>0</v>
+      </c>
+      <c r="H19" s="114">
+        <v>0</v>
+      </c>
+      <c r="I19" s="115" t="s">
+        <v>98</v>
+      </c>
       <c r="K19" s="9"/>
       <c r="M19" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N19" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O19" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11744,16 +11770,22 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F19),"",'Sprint 1 - Bilan'!F19)</f>
         <v/>
       </c>
-      <c r="G20" s="110"/>
-      <c r="H20" s="111"/>
-      <c r="I20" s="112"/>
+      <c r="G20" s="110">
+        <v>0</v>
+      </c>
+      <c r="H20" s="111">
+        <v>0</v>
+      </c>
+      <c r="I20" s="115" t="s">
+        <v>98</v>
+      </c>
       <c r="M20" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N20" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O20" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11786,16 +11818,22 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F20),"",'Sprint 1 - Bilan'!F20)</f>
         <v/>
       </c>
-      <c r="G21" s="116"/>
-      <c r="H21" s="114"/>
-      <c r="I21" s="115"/>
+      <c r="G21" s="116">
+        <v>0</v>
+      </c>
+      <c r="H21" s="114">
+        <v>0</v>
+      </c>
+      <c r="I21" s="115" t="s">
+        <v>98</v>
+      </c>
       <c r="M21" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O21" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11875,7 +11913,7 @@
         <v/>
       </c>
       <c r="G23" s="113">
-        <v>4.1666666666666699E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H23" s="114">
         <v>1</v>
@@ -12742,15 +12780,15 @@
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M44" s="3">
         <f>COUNTIF(M9:M43,TRUE)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N44" s="3">
         <f t="shared" ref="N44:O44" si="5">COUNTIF(N9:N43,TRUE)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O44" s="3">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P44" s="3">
         <f>COUNTIF(P9:P43,FALSE)</f>
@@ -12761,14 +12799,14 @@
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M45" s="3">
         <f>SUM(M44:O44)</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="R45" s="8"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M46" s="3" t="str">
         <f>IF(M45=0, "aucun champ", IF(M45=1, "1 champ", M45 &amp; " champs"))</f>
-        <v>11 champs</v>
+        <v>aucun champ</v>
       </c>
       <c r="R46" s="8"/>
     </row>
@@ -12826,7 +12864,7 @@
       <formula>OR($D9="Sprint 3",AND($D9="Sprint 1",$F9=100%))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G21:I21 G23:I23 G25:I25 G27:I27 G29:I29 G31:I31 G33:I33 G35:I35 G37:I37 G39:I39 G41:I41 G43:I43">
+  <conditionalFormatting sqref="G21:H21 G23:I23 G25:I25 G27:I27 G29:I29 G31:I31 G33:I33 G35:I35 G37:I37 G39:I39 G41:I41 G43:I43">
     <cfRule type="expression" dxfId="33" priority="19">
       <formula>AND($D21="Sprint 3",$H21&gt;0)</formula>
     </cfRule>
@@ -12834,7 +12872,7 @@
       <formula>AND($D21&lt;&gt;"Sprint 3",$H21&lt;1,NOT(ISBLANK($H21)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20:I20 G22:I22 G24:I24 G26:I26 G28:I28 G30:I30 G32:I32 G34:I34 G36:I36 G38:I38 G40:I40 G42:I42">
+  <conditionalFormatting sqref="G20:H20 G22:I22 G24:I24 G26:I26 G28:I28 G30:I30 G32:I32 G34:I34 G36:I36 G38:I38 G40:I40 G42:I42">
     <cfRule type="expression" dxfId="31" priority="16">
       <formula>AND($D20="Sprint 3",$H20&gt;0)</formula>
     </cfRule>
@@ -12842,9 +12880,9 @@
       <formula>AND($D20&lt;&gt;"Sprint 3",$H20&lt;1,NOT(ISBLANK($H20)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:I43">
+  <conditionalFormatting sqref="I22:I43">
     <cfRule type="expression" dxfId="29" priority="15">
-      <formula>$O20</formula>
+      <formula>$O22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20:G43">
@@ -12862,54 +12900,54 @@
       <formula>$M$45&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:F9 B11:F11 B13:F13 B15:F15 B17:F17 B19:F19 B21:I21 B23:I23 B25:I25 B27:I27 B29:I29 B31:I31 B33:I33 B35:I35 B37:I37 B39:I39 B41:I41 B43:I43">
+  <conditionalFormatting sqref="B9:F9 B11:F11 B13:F13 B15:F15 B17:F17 B19:F19 B21:H21 B23:I23 B25:I25 B27:I27 B29:I29 B31:I31 B33:I33 B35:I35 B37:I37 B39:I39 B41:I41 B43:I43">
     <cfRule type="expression" dxfId="25" priority="21">
       <formula>LEN($B9)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10:F10 B12:F12 B14:F14 B16:F16 B18:F18 B20:I20 B22:I22 B24:I24 B26:I26 B28:I28 B30:I30 B32:I32 B34:I34 B36:I36 B38:I38 B40:I40 B42:I42">
+  <conditionalFormatting sqref="B10:F10 B12:F12 B14:F14 B16:F16 B18:F18 B20:H20 B22:I22 B24:I24 B26:I26 B28:I28 B30:I30 B32:I32 B34:I34 B36:I36 B38:I38 B40:I40 B42:I42">
     <cfRule type="expression" dxfId="24" priority="18">
       <formula>LEN($B10)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G9:I9 G11:I11 G13:I13 G15:I15 G17:I17 G19:I19">
-    <cfRule type="expression" dxfId="23" priority="7">
+  <conditionalFormatting sqref="G9:I9 G11:I11 G13:I13 G15:I15 G17:I17 G19:H19 I18:I21">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>AND($D9="Sprint 3",$H9&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="8">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>AND($D9&lt;&gt;"Sprint 3",$H9&lt;1,NOT(ISBLANK($H9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G10:I10 G12:I12 G14:I14 G16:I16 G18:I18">
-    <cfRule type="expression" dxfId="21" priority="4">
+  <conditionalFormatting sqref="G10:I10 G12:I12 G14:I14 G16:I16 G18:H18">
+    <cfRule type="expression" dxfId="23" priority="4">
       <formula>AND($D10="Sprint 3",$H10&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="5">
+    <cfRule type="expression" dxfId="22" priority="5">
       <formula>AND($D10&lt;&gt;"Sprint 3",$H10&lt;1,NOT(ISBLANK($H10)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9:I19">
-    <cfRule type="expression" dxfId="19" priority="3">
+  <conditionalFormatting sqref="I9:I21">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>$O9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:G19">
-    <cfRule type="expression" dxfId="18" priority="2">
+    <cfRule type="expression" dxfId="21" priority="2">
       <formula>$M9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H19">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="20" priority="1">
       <formula>$N9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G9:I9 G11:I11 G13:I13 G15:I15 G17:I17 G19:I19">
-    <cfRule type="expression" dxfId="16" priority="9">
+  <conditionalFormatting sqref="G9:I9 G11:I11 G13:I13 G15:I15 G17:I17 G19:H19 I18:I21">
+    <cfRule type="expression" dxfId="0" priority="9">
       <formula>LEN($B9)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G10:I10 G12:I12 G14:I14 G16:I16 G18:I18">
-    <cfRule type="expression" dxfId="15" priority="6">
+  <conditionalFormatting sqref="G10:I10 G12:I12 G14:I14 G16:I16 G18:H18">
+    <cfRule type="expression" dxfId="19" priority="6">
       <formula>LEN($B10)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12944,7 +12982,7 @@
   <dimension ref="B1:Z57"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13283,7 +13321,7 @@
       </c>
       <c r="E13" s="73">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E13)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G13)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E13)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G13))</f>
-        <v>4.1666666666666699E-2</v>
+        <v>8.3333333333333301E-2</v>
       </c>
       <c r="F13" s="77">
         <f>IF(LEN('Sprint 2 - Bilan'!$H13)&lt;&gt;0,'Sprint 2 - Bilan'!$H13,IF(LEN('Sprint 2 - Bilan'!$F13)=0,"",'Sprint 2 - Bilan'!$F13))</f>
@@ -13389,7 +13427,7 @@
       </c>
       <c r="E15" s="73">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E15)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G15)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E15)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G15))</f>
-        <v>4.1666666666666699E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F15" s="77">
         <f>IF(LEN('Sprint 2 - Bilan'!$H15)&lt;&gt;0,'Sprint 2 - Bilan'!$H15,IF(LEN('Sprint 2 - Bilan'!$F15)=0,"",'Sprint 2 - Bilan'!$F15))</f>
@@ -13491,9 +13529,9 @@
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E17)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G17)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E17)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G17))</f>
         <v/>
       </c>
-      <c r="F17" s="76" t="str">
+      <c r="F17" s="76">
         <f>IF(LEN('Sprint 2 - Bilan'!$H17)&lt;&gt;0,'Sprint 2 - Bilan'!$H17,IF(LEN('Sprint 2 - Bilan'!$F17)=0,"",'Sprint 2 - Bilan'!$F17))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="G17" s="113"/>
       <c r="H17" s="114"/>
@@ -13533,9 +13571,9 @@
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E18)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G18)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E18)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G18))</f>
         <v/>
       </c>
-      <c r="F18" s="75" t="str">
+      <c r="F18" s="75">
         <f>IF(LEN('Sprint 2 - Bilan'!$H18)&lt;&gt;0,'Sprint 2 - Bilan'!$H18,IF(LEN('Sprint 2 - Bilan'!$F18)=0,"",'Sprint 2 - Bilan'!$F18))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="G18" s="110"/>
       <c r="H18" s="111"/>
@@ -13575,9 +13613,9 @@
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E19)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G19)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E19)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G19))</f>
         <v/>
       </c>
-      <c r="F19" s="77" t="str">
+      <c r="F19" s="77">
         <f>IF(LEN('Sprint 2 - Bilan'!$H19)&lt;&gt;0,'Sprint 2 - Bilan'!$H19,IF(LEN('Sprint 2 - Bilan'!$F19)=0,"",'Sprint 2 - Bilan'!$F19))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="G19" s="116"/>
       <c r="H19" s="114"/>
@@ -13617,9 +13655,9 @@
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E20)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G20)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E20)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G20))</f>
         <v/>
       </c>
-      <c r="F20" s="75" t="str">
+      <c r="F20" s="75">
         <f>IF(LEN('Sprint 2 - Bilan'!$H20)&lt;&gt;0,'Sprint 2 - Bilan'!$H20,IF(LEN('Sprint 2 - Bilan'!$F20)=0,"",'Sprint 2 - Bilan'!$F20))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="G20" s="110"/>
       <c r="H20" s="111"/>
@@ -13659,9 +13697,9 @@
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E21)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G21)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E21)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G21))</f>
         <v/>
       </c>
-      <c r="F21" s="77" t="str">
+      <c r="F21" s="77">
         <f>IF(LEN('Sprint 2 - Bilan'!$H21)&lt;&gt;0,'Sprint 2 - Bilan'!$H21,IF(LEN('Sprint 2 - Bilan'!$F21)=0,"",'Sprint 2 - Bilan'!$F21))</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="G21" s="116"/>
       <c r="H21" s="114"/>
@@ -13741,7 +13779,7 @@
       </c>
       <c r="E23" s="72">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E23)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G23)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E23)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G23))</f>
-        <v>4.1666666666666699E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F23" s="76">
         <f>IF(LEN('Sprint 2 - Bilan'!$H23)&lt;&gt;0,'Sprint 2 - Bilan'!$H23,IF(LEN('Sprint 2 - Bilan'!$F23)=0,"",'Sprint 2 - Bilan'!$F23))</f>
@@ -14688,50 +14726,50 @@
     <mergeCell ref="I7:I8"/>
   </mergeCells>
   <conditionalFormatting sqref="B9:F43">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>OR($F9=100%,$H9=100%)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>AND($D9&lt;&gt;"Sprint 3",$F9=100%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:I9 G11:I11 G13:I13 G15:I15 G17:I17 G19:I19 G21:I21 G23:I23 G25:I25 G27:I27 G29:I29 G31:I31 G33:I33 G35:I35 G37:I37 G39:I39 G41:I41 G43:I43">
-    <cfRule type="expression" dxfId="12" priority="11">
+    <cfRule type="expression" dxfId="16" priority="11">
       <formula>IF(ISBLANK($H9),IF(ISBLANK($F9),TRUE,$F9&lt;100%),$H9&lt;100%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:I10 G12:I12 G14:I14 G16:I16 G18:I18 G20:I20 G22:I22 G24:I24 G26:I26 G28:I28 G30:I30 G32:I32 G34:I34 G36:I36 G38:I38 G40:I40 G42:I42">
-    <cfRule type="expression" dxfId="11" priority="8">
+    <cfRule type="expression" dxfId="15" priority="8">
       <formula>IF(ISBLANK($H10),IF(ISBLANK($F10),TRUE,$F10&lt;100%),$H10&lt;100%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I43">
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="14" priority="6">
       <formula>$O9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:G43">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="13" priority="5">
       <formula>$M9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H43">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>$N9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>$M$45&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:I9 B11:I11 B13:I13 B15:I15 B17:I17 B19:I19 B21:I21 B23:I23 B25:I25 B27:I27 B29:I29 B31:I31 B33:I33 B35:I35 B37:I37 B39:I39 B41:I41 B43:I43">
-    <cfRule type="expression" dxfId="6" priority="12">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>LEN($B9)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:I10 B12:I12 B14:I14 B16:I16 B18:I18 B20:I20 B22:I22 B24:I24 B26:I26 B28:I28 B30:I30 B32:I32 B34:I34 B36:I36 B38:I38 B40:I40 B42:I42">
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>LEN($B10)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14947,7 +14985,7 @@
       </c>
       <c r="V9" s="2">
         <f>COUNTIF('Sprint 1 - Planification'!E8:E42,"Essentielle")</f>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="X9" s="2" t="s">
         <v>69</v>
@@ -14967,7 +15005,7 @@
       </c>
       <c r="D10" s="94" t="str">
         <f t="shared" si="0"/>
-        <v>16h00</v>
+        <v>18h00</v>
       </c>
       <c r="E10" s="95" t="str">
         <f t="shared" si="0"/>
@@ -14975,7 +15013,7 @@
       </c>
       <c r="F10" s="99" t="str">
         <f t="shared" si="0"/>
-        <v>28h00</v>
+        <v>30h00</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -14985,7 +15023,7 @@
       </c>
       <c r="M10" s="1">
         <f>'Sprint 2 - Bilan'!V9</f>
-        <v>0.66666666666666818</v>
+        <v>0.75000000000000133</v>
       </c>
       <c r="N10" s="1">
         <f>'Sprint 3 - Bilan'!V9</f>
@@ -14993,7 +15031,7 @@
       </c>
       <c r="O10" s="1">
         <f>SUM(L10:N10)</f>
-        <v>1.1666666666666679</v>
+        <v>1.2500000000000009</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>66</v>
@@ -15004,7 +15042,7 @@
       </c>
       <c r="R10" s="1">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="S10" s="1">
         <f t="shared" si="1"/>
@@ -15015,7 +15053,7 @@
       </c>
       <c r="V10" s="2">
         <f>COUNTIF('Sprint 1 - Planification'!E8:E42,"Optionnelle")</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="X10" s="2" t="s">
         <v>70</v>
@@ -15194,7 +15232,7 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="ZTHIqTmr8cTliRMGAcUcmM0mjbf6CIJ0mHH1g8KtGLF4lRA/UYuFPwpT4A16q2cQqIx/6PesESjQGKIAV9ov5g==" saltValue="9FKXXuq3MsinQZgjNrQSTw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <conditionalFormatting sqref="F5:J5">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15517,22 +15555,22 @@
     <mergeCell ref="C35:G35"/>
   </mergeCells>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="3" priority="69">
+    <cfRule type="expression" dxfId="7" priority="69">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>